<commit_message>
GDE-8514 Update Create Customer
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="10" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="14" activeTab="17" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Batch_EOD" sheetId="1" state="visible" r:id="rId1"/>
@@ -1538,7 +1538,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1515030</t>
+          <t>137</t>
         </is>
       </c>
       <c r="R2" s="59" t="inlineStr">
@@ -2571,8 +2571,8 @@
     <col width="40.85546875" bestFit="1" customWidth="1" style="78" min="26" max="26"/>
     <col width="16.7109375" bestFit="1" customWidth="1" style="78" min="27" max="27"/>
     <col width="19.85546875" bestFit="1" customWidth="1" style="78" min="28" max="28"/>
-    <col width="9.140625" customWidth="1" style="78" min="29" max="82"/>
-    <col width="9.140625" customWidth="1" style="78" min="83" max="16384"/>
+    <col width="9.140625" customWidth="1" style="78" min="29" max="84"/>
+    <col width="9.140625" customWidth="1" style="78" min="85" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="73" thickBot="1">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="AV2" s="51" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>137</t>
         </is>
       </c>
       <c r="AW2" s="51" t="inlineStr">
@@ -3622,7 +3622,7 @@
   </sheetPr>
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -3660,8 +3660,8 @@
     <col width="18.42578125" bestFit="1" customWidth="1" style="104" min="31" max="31"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="104" min="32" max="32"/>
     <col width="20.85546875" bestFit="1" customWidth="1" style="104" min="33" max="33"/>
-    <col width="9" customWidth="1" style="104" min="34" max="77"/>
-    <col width="9" customWidth="1" style="104" min="78" max="16384"/>
+    <col width="9" customWidth="1" style="104" min="34" max="79"/>
+    <col width="9" customWidth="1" style="104" min="80" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="99" thickBot="1">
@@ -4683,8 +4683,8 @@
   </sheetPr>
   <dimension ref="A1:BQ9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="BB2" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>137</t>
         </is>
       </c>
       <c r="BC2" s="54" t="inlineStr">
@@ -5364,11 +5364,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB5"/>
+  <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW21" sqref="AW21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BC1" sqref="BC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -5700,6 +5700,11 @@
           <t>Borrower1_NoticeMethod</t>
         </is>
       </c>
+      <c r="BC1" s="88" t="inlineStr">
+        <is>
+          <t>LIQCustomer_ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5958,6 +5963,11 @@
       <c r="BB2" t="inlineStr">
         <is>
           <t>CBA Email with PDF Attachment</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>137</t>
         </is>
       </c>
     </row>
@@ -6256,8 +6266,8 @@
   </sheetPr>
   <dimension ref="A1:CR2"/>
   <sheetViews>
-    <sheetView topLeftCell="BR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT5" sqref="BT5"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -6888,16 +6898,18 @@
       </c>
       <c r="L2" s="58" t="inlineStr">
         <is>
-          <t>ESPS11413431</t>
+          <t>IEEBRW7642S524118</t>
         </is>
       </c>
       <c r="M2" s="58" t="inlineStr">
         <is>
-          <t>ESPS11413431</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>1413434</v>
+          <t>IEEBRW7642S524119</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="O2" s="52" t="n"/>
       <c r="P2" s="52" t="n"/>

</xml_diff>

<commit_message>
GDE-8513 Update Search Customer
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="14" activeTab="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Batch_EOD" sheetId="1" state="visible" r:id="rId1"/>
@@ -246,7 +246,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -415,6 +415,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2571,8 +2572,8 @@
     <col width="40.85546875" bestFit="1" customWidth="1" style="78" min="26" max="26"/>
     <col width="16.7109375" bestFit="1" customWidth="1" style="78" min="27" max="27"/>
     <col width="19.85546875" bestFit="1" customWidth="1" style="78" min="28" max="28"/>
-    <col width="9.140625" customWidth="1" style="78" min="29" max="84"/>
-    <col width="9.140625" customWidth="1" style="78" min="85" max="16384"/>
+    <col width="9.140625" customWidth="1" style="78" min="29" max="90"/>
+    <col width="9.140625" customWidth="1" style="78" min="91" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="73" thickBot="1">
@@ -3660,8 +3661,8 @@
     <col width="18.42578125" bestFit="1" customWidth="1" style="104" min="31" max="31"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="104" min="32" max="32"/>
     <col width="20.85546875" bestFit="1" customWidth="1" style="104" min="33" max="33"/>
-    <col width="9" customWidth="1" style="104" min="34" max="79"/>
-    <col width="9" customWidth="1" style="104" min="80" max="16384"/>
+    <col width="9" customWidth="1" style="104" min="34" max="85"/>
+    <col width="9" customWidth="1" style="104" min="86" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="99" thickBot="1">
@@ -5366,7 +5367,7 @@
   </sheetPr>
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BC1" sqref="BC1"/>
     </sheetView>
@@ -6264,10 +6265,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CR2"/>
+  <dimension ref="A1:DL2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -6354,6 +6355,24 @@
     <col width="43.85546875" customWidth="1" style="1" min="94" max="94"/>
     <col width="48.85546875" customWidth="1" style="1" min="95" max="95"/>
     <col width="34.85546875" customWidth="1" style="1" min="96" max="96"/>
+    <col width="28" bestFit="1" customWidth="1" style="1" min="97" max="97"/>
+    <col width="6" bestFit="1" customWidth="1" style="1" min="98" max="98"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="1" min="99" max="99"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="1" min="100" max="100"/>
+    <col width="22" bestFit="1" customWidth="1" style="1" min="101" max="101"/>
+    <col width="21" bestFit="1" customWidth="1" style="1" min="102" max="102"/>
+    <col width="29.85546875" bestFit="1" customWidth="1" style="1" min="103" max="103"/>
+    <col width="28.7109375" bestFit="1" customWidth="1" style="1" min="104" max="104"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" style="1" min="105" max="105"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" style="1" min="106" max="106"/>
+    <col width="26" bestFit="1" customWidth="1" style="1" min="107" max="107"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="1" min="108" max="108"/>
+    <col width="21.5703125" bestFit="1" customWidth="1" style="1" min="109" max="109"/>
+    <col width="19.140625" bestFit="1" customWidth="1" style="1" min="110" max="110"/>
+    <col width="35.7109375" bestFit="1" customWidth="1" style="1" min="111" max="111"/>
+    <col width="34.28515625" bestFit="1" customWidth="1" style="1" min="112" max="113"/>
+    <col width="31.7109375" bestFit="1" customWidth="1" style="1" min="114" max="114"/>
+    <col width="32.5703125" bestFit="1" customWidth="1" style="1" min="116" max="116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="18">
@@ -6837,6 +6856,106 @@
       <c r="CR1" s="19" t="inlineStr">
         <is>
           <t>RemittanceInstructionSIMT_AutoDoIt</t>
+        </is>
+      </c>
+      <c r="CS1" s="89" t="inlineStr">
+        <is>
+          <t>CustomerNotice_TypeMethod</t>
+        </is>
+      </c>
+      <c r="CT1" s="89" t="inlineStr">
+        <is>
+          <t>Entity</t>
+        </is>
+      </c>
+      <c r="CU1" s="89" t="inlineStr">
+        <is>
+          <t>CustomerSourceApp</t>
+        </is>
+      </c>
+      <c r="CV1" s="89" t="inlineStr">
+        <is>
+          <t>BorrowerContact_Phone</t>
+        </is>
+      </c>
+      <c r="CW1" s="89" t="inlineStr">
+        <is>
+          <t>ProductSBLC_Checkbox</t>
+        </is>
+      </c>
+      <c r="CX1" s="89" t="inlineStr">
+        <is>
+          <t>ProductLoan_Checkbox</t>
+        </is>
+      </c>
+      <c r="CY1" s="89" t="inlineStr">
+        <is>
+          <t>BalanceType_Principal_Checkbox</t>
+        </is>
+      </c>
+      <c r="CZ1" s="89" t="inlineStr">
+        <is>
+          <t>BalanceType_Interest_Checkbox</t>
+        </is>
+      </c>
+      <c r="DA1" s="89" t="inlineStr">
+        <is>
+          <t>BalanceType_Fees_Checkbox</t>
+        </is>
+      </c>
+      <c r="DB1" s="89" t="inlineStr">
+        <is>
+          <t>Address_Code</t>
+        </is>
+      </c>
+      <c r="DC1" s="89" t="inlineStr">
+        <is>
+          <t>RI_ProductLoan_Checkbox</t>
+        </is>
+      </c>
+      <c r="DD1" s="89" t="inlineStr">
+        <is>
+          <t>RI_ProductSBLC_Checkbox</t>
+        </is>
+      </c>
+      <c r="DE1" s="89" t="inlineStr">
+        <is>
+          <t>RI_FromCust_Checkbox</t>
+        </is>
+      </c>
+      <c r="DF1" s="89" t="inlineStr">
+        <is>
+          <t>RI_ToCust_Checkbox</t>
+        </is>
+      </c>
+      <c r="DG1" s="89" t="inlineStr">
+        <is>
+          <t>RI_BalanceType_Principal_Checkbox</t>
+        </is>
+      </c>
+      <c r="DH1" s="89" t="inlineStr">
+        <is>
+          <t>RI_BalanceType_Interest_Checkbox</t>
+        </is>
+      </c>
+      <c r="DI1" s="89" t="inlineStr">
+        <is>
+          <t>RI_BalanceType_Fees_Checkbox</t>
+        </is>
+      </c>
+      <c r="DJ1" s="89" t="inlineStr">
+        <is>
+          <t>RI_BalanceType_Fees_Checkbox</t>
+        </is>
+      </c>
+      <c r="DK1" s="89" t="inlineStr">
+        <is>
+          <t>RI_AutoDoIt_Checkbox</t>
+        </is>
+      </c>
+      <c r="DL1" s="89" t="inlineStr">
+        <is>
+          <t>RI_SendersCorrespondent_Checkbox</t>
         </is>
       </c>
     </row>
@@ -6919,7 +7038,7 @@
       <c r="T2" s="52" t="n"/>
       <c r="U2" s="58" t="inlineStr">
         <is>
-          <t>DDA1</t>
+          <t>DDAAUD1-4156</t>
         </is>
       </c>
       <c r="V2" s="58" t="n"/>
@@ -6930,7 +7049,7 @@
       </c>
       <c r="Y2" s="58" t="inlineStr">
         <is>
-          <t>RTGS1</t>
+          <t>RTGSAUD1-4159</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -7011,7 +7130,7 @@
       </c>
       <c r="AS2" s="52" t="inlineStr">
         <is>
-          <t>FORG</t>
+          <t>BFPR</t>
         </is>
       </c>
       <c r="AT2" s="52" t="inlineStr">
@@ -7185,6 +7304,11 @@
           <t>International Money Transfer</t>
         </is>
       </c>
+      <c r="CG2" t="inlineStr">
+        <is>
+          <t>IMTUSD1-4158</t>
+        </is>
+      </c>
       <c r="CI2" s="51" t="inlineStr">
         <is>
           <t>USD</t>
@@ -7233,6 +7357,106 @@
       <c r="CR2" s="52" t="inlineStr">
         <is>
           <t>&lt;Selected&gt;</t>
+        </is>
+      </c>
+      <c r="CS2" s="58" t="inlineStr">
+        <is>
+          <t>Faxes/Emails Only</t>
+        </is>
+      </c>
+      <c r="CT2" s="52" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="CU2" s="58" t="inlineStr">
+        <is>
+          <t>LIQ</t>
+        </is>
+      </c>
+      <c r="CV2" s="124" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="CW2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="CX2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="CY2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="CZ2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DA2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DB2" s="52" t="inlineStr">
+        <is>
+          <t>LEGAL ADDRESS</t>
+        </is>
+      </c>
+      <c r="DC2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DD2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DE2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DF2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DG2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DH2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DI2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DJ2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="DK2" s="58" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="DL2" s="58" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-8513 Update Secondary Sale
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="12" activeTab="17" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Batch_EOD" sheetId="1" state="visible" r:id="rId1"/>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" s="54" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2380,12 +2380,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="68" t="inlineStr">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>60000263</t>
+          <t>60001298</t>
         </is>
       </c>
       <c r="G2" s="116" t="inlineStr">
@@ -2572,8 +2572,8 @@
     <col width="40.85546875" bestFit="1" customWidth="1" style="78" min="26" max="26"/>
     <col width="16.7109375" bestFit="1" customWidth="1" style="78" min="27" max="27"/>
     <col width="19.85546875" bestFit="1" customWidth="1" style="78" min="28" max="28"/>
-    <col width="9.140625" customWidth="1" style="78" min="29" max="90"/>
-    <col width="9.140625" customWidth="1" style="78" min="91" max="16384"/>
+    <col width="9.140625" customWidth="1" style="78" min="29" max="95"/>
+    <col width="9.140625" customWidth="1" style="78" min="96" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="73" thickBot="1">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="53" t="inlineStr">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>06-Sep-2021</t>
+          <t>06-Jun-2022</t>
         </is>
       </c>
       <c r="L2" s="53" t="inlineStr">
@@ -3661,8 +3661,8 @@
     <col width="18.42578125" bestFit="1" customWidth="1" style="104" min="31" max="31"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="104" min="32" max="32"/>
     <col width="20.85546875" bestFit="1" customWidth="1" style="104" min="33" max="33"/>
-    <col width="9" customWidth="1" style="104" min="34" max="85"/>
-    <col width="9" customWidth="1" style="104" min="86" max="16384"/>
+    <col width="9" customWidth="1" style="104" min="34" max="90"/>
+    <col width="9" customWidth="1" style="104" min="91" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="99" thickBot="1">
@@ -3845,12 +3845,12 @@
       </c>
       <c r="C2" s="58" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="103" t="inlineStr">
@@ -4101,8 +4101,8 @@
   </sheetPr>
   <dimension ref="A1:AT11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="C2:D2"/>
+    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4397,12 +4397,12 @@
       </c>
       <c r="C2" s="58" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="51" t="inlineStr">
@@ -4427,7 +4427,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>60000263</t>
+          <t>60001298</t>
         </is>
       </c>
       <c r="J2" s="53" t="inlineStr">
@@ -4437,12 +4437,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="M2" s="53" t="inlineStr">
@@ -4482,12 +4482,12 @@
       </c>
       <c r="T2" s="53" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>07-Aug-2021</t>
+          <t>07-May-2022</t>
         </is>
       </c>
       <c r="V2" s="58" t="inlineStr">
@@ -4522,7 +4522,7 @@
       </c>
       <c r="AB2" s="51" t="inlineStr">
         <is>
-          <t>CB001/Hold for Investment - Australia/BG_COL</t>
+          <t>CB001/Hold for Investment - Australia/BP_COL</t>
         </is>
       </c>
       <c r="AC2" s="51" t="n">
@@ -5096,7 +5096,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" s="54" t="inlineStr">
@@ -5106,7 +5106,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5367,9 +5367,9 @@
   </sheetPr>
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BC1" sqref="BC1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -5720,12 +5720,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -5745,7 +5745,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ONG000000000285</t>
+          <t>ONG000000000742</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -5953,7 +5953,7 @@
       </c>
       <c r="AZ2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="BA2" t="inlineStr">
@@ -6160,27 +6160,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>08-Jul-2020</t>
+          <t>07-Apr-2021</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>06-Sep-2020</t>
+          <t>06-Jun-2021</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>09-Sep-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="H2" s="59" t="inlineStr">
@@ -6267,7 +6267,7 @@
   </sheetPr>
   <dimension ref="A1:DL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AN4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -7926,12 +7926,12 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>60000263</t>
+          <t>60001298</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>60000274</t>
+          <t>60001303</t>
         </is>
       </c>
       <c r="AT2" t="inlineStr">
@@ -8117,8 +8117,8 @@
   <dimension ref="A1:EV19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G2" sqref="G2"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -9044,17 +9044,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>S517082020175355MVH</t>
+          <t>S526102020092403AYH</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="I2" s="56" t="inlineStr">
@@ -9445,12 +9445,12 @@
       </c>
       <c r="DH2" t="inlineStr">
         <is>
-          <t>07-Aug-2021</t>
+          <t>07-May-2022</t>
         </is>
       </c>
       <c r="DI2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="DK2" t="inlineStr">
@@ -9505,12 +9505,12 @@
       </c>
       <c r="DU2" s="58" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="DV2" s="58" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="DW2" s="53" t="inlineStr">
@@ -9575,7 +9575,7 @@
       </c>
       <c r="EI2" s="58" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="EJ2" s="61" t="n"/>
@@ -9960,12 +9960,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -10690,7 +10690,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="56" t="inlineStr">
@@ -10883,7 +10883,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -11018,7 +11018,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" s="56" t="inlineStr">
@@ -11034,7 +11034,7 @@
       <c r="F2" s="59" t="n"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="H2" s="59" t="inlineStr">
@@ -11044,12 +11044,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="K2" s="59" t="n"/>
@@ -11249,12 +11249,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" s="58" t="inlineStr">
@@ -11304,14 +11304,14 @@
       <c r="O2" s="59" t="n"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-May-2021</t>
         </is>
       </c>
       <c r="Q2" s="59" t="n"/>
       <c r="R2" s="59" t="n"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>07-Aug-2021</t>
+          <t>07-May-2022</t>
         </is>
       </c>
     </row>
@@ -11536,17 +11536,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_17082020175353QDI</t>
+          <t>BNS5_26102020092357SDC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM17082020181303GHY</t>
+          <t>S5TERM26102020100203HRK</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>60000274</t>
+          <t>60001303</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
GDE-8513 Update Components for Scenario 5 Hotfix
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ05_SecondarySale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="780" firstSheet="12" activeTab="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3600" yWindow="1830" windowWidth="21600" windowHeight="11385" tabRatio="780" firstSheet="6" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Batch_EOD" sheetId="1" state="visible" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>147</t>
         </is>
       </c>
       <c r="R2" s="59" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" s="54" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2380,12 +2380,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="68" t="inlineStr">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>60001298</t>
+          <t>60001332</t>
         </is>
       </c>
       <c r="G2" s="116" t="inlineStr">
@@ -2572,8 +2572,8 @@
     <col width="40.85546875" bestFit="1" customWidth="1" style="78" min="26" max="26"/>
     <col width="16.7109375" bestFit="1" customWidth="1" style="78" min="27" max="27"/>
     <col width="19.85546875" bestFit="1" customWidth="1" style="78" min="28" max="28"/>
-    <col width="9.140625" customWidth="1" style="78" min="29" max="95"/>
-    <col width="9.140625" customWidth="1" style="78" min="96" max="16384"/>
+    <col width="9.140625" customWidth="1" style="78" min="29" max="99"/>
+    <col width="9.140625" customWidth="1" style="78" min="100" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="73" thickBot="1">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="53" t="inlineStr">
@@ -3237,12 +3237,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>10-Sep-2020</t>
+          <t>15-Sep-2021</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>06-Jun-2022</t>
+          <t>11-Sep-2022</t>
         </is>
       </c>
       <c r="L2" s="53" t="inlineStr">
@@ -3267,7 +3267,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>60000538</t>
+          <t>60001338</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>650.00</t>
+          <t>700.00</t>
         </is>
       </c>
       <c r="AE2" s="52" t="inlineStr">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="AV2" s="51" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>147</t>
         </is>
       </c>
       <c r="AW2" s="51" t="inlineStr">
@@ -3661,8 +3661,8 @@
     <col width="18.42578125" bestFit="1" customWidth="1" style="104" min="31" max="31"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="104" min="32" max="32"/>
     <col width="20.85546875" bestFit="1" customWidth="1" style="104" min="33" max="33"/>
-    <col width="9" customWidth="1" style="104" min="34" max="90"/>
-    <col width="9" customWidth="1" style="104" min="91" max="16384"/>
+    <col width="9" customWidth="1" style="104" min="34" max="94"/>
+    <col width="9" customWidth="1" style="104" min="95" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customFormat="1" customHeight="1" s="99" thickBot="1">
@@ -3845,12 +3845,12 @@
       </c>
       <c r="C2" s="58" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="103" t="inlineStr">
@@ -3858,12 +3858,14 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>60000538</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>60001338</t>
+        </is>
       </c>
       <c r="G2" s="104" t="inlineStr">
         <is>
-          <t>60000646</t>
+          <t>60001346</t>
         </is>
       </c>
       <c r="H2" s="105" t="n">
@@ -4397,12 +4399,12 @@
       </c>
       <c r="C2" s="58" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="51" t="inlineStr">
@@ -4427,7 +4429,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>60001298</t>
+          <t>60001332</t>
         </is>
       </c>
       <c r="J2" s="53" t="inlineStr">
@@ -4437,12 +4439,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="M2" s="53" t="inlineStr">
@@ -4482,12 +4484,12 @@
       </c>
       <c r="T2" s="53" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>07-May-2022</t>
+          <t>12-Aug-2022</t>
         </is>
       </c>
       <c r="V2" s="58" t="inlineStr">
@@ -5096,7 +5098,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" s="54" t="inlineStr">
@@ -5106,7 +5108,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5272,7 +5274,7 @@
       </c>
       <c r="BB2" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>147</t>
         </is>
       </c>
       <c r="BC2" s="54" t="inlineStr">
@@ -5365,11 +5367,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC5"/>
+  <dimension ref="A1:BD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -5706,6 +5708,11 @@
           <t>LIQCustomer_ID</t>
         </is>
       </c>
+      <c r="BD1" s="90" t="inlineStr">
+        <is>
+          <t>Days</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5720,12 +5727,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -5745,7 +5752,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ONG000000000742</t>
+          <t>ONG000000000746</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -5770,7 +5777,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>08-Sep-2020</t>
+          <t>13-Sep-2021</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -5784,7 +5791,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>18.33</v>
+        <v>87.67</v>
       </c>
       <c r="Q2" s="17" t="n">
         <v>100000</v>
@@ -5842,17 +5849,17 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>14-Aug-2020</t>
+          <t>13-Sep-2021</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>15-Jul-2020</t>
+          <t>14-Aug-2021</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>13-Sep-2020</t>
+          <t>13-Oct-2021</t>
         </is>
       </c>
       <c r="AF2" s="59" t="inlineStr">
@@ -5953,7 +5960,7 @@
       </c>
       <c r="AZ2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="BA2" t="inlineStr">
@@ -5968,8 +5975,11 @@
       </c>
       <c r="BC2" t="inlineStr">
         <is>
-          <t>137</t>
-        </is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="BD2" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -6160,27 +6170,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>07-Apr-2021</t>
+          <t>13-Jul-2021</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>06-Jun-2021</t>
+          <t>11-Sep-2021</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>13-Sep-2021</t>
         </is>
       </c>
       <c r="H2" s="59" t="inlineStr">
@@ -7017,17 +7027,17 @@
       </c>
       <c r="L2" s="58" t="inlineStr">
         <is>
-          <t>IEEBRW7642S524118</t>
+          <t>IEEBRW7642S542122</t>
         </is>
       </c>
       <c r="M2" s="58" t="inlineStr">
         <is>
-          <t>IEEBRW7642S524119</t>
+          <t>IEEBRW7642S542123</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>147</t>
         </is>
       </c>
       <c r="O2" s="52" t="n"/>
@@ -7038,7 +7048,7 @@
       <c r="T2" s="52" t="n"/>
       <c r="U2" s="58" t="inlineStr">
         <is>
-          <t>DDAAUD1-4156</t>
+          <t>DDAAUD1-4835</t>
         </is>
       </c>
       <c r="V2" s="58" t="n"/>
@@ -7049,7 +7059,7 @@
       </c>
       <c r="Y2" s="58" t="inlineStr">
         <is>
-          <t>RTGSAUD1-4159</t>
+          <t>RTGSAUD1-4838</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -7306,7 +7316,7 @@
       </c>
       <c r="CG2" t="inlineStr">
         <is>
-          <t>IMTUSD1-4158</t>
+          <t>IMTUSD1-4837</t>
         </is>
       </c>
       <c r="CI2" s="51" t="inlineStr">
@@ -7781,7 +7791,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -7926,12 +7936,12 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>60001298</t>
+          <t>60001332</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>60001303</t>
+          <t>60001334</t>
         </is>
       </c>
       <c r="AT2" t="inlineStr">
@@ -9044,17 +9054,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>S526102020092403AYH</t>
+          <t>S529102020093009FSF</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="I2" s="56" t="inlineStr">
@@ -9445,12 +9455,12 @@
       </c>
       <c r="DH2" t="inlineStr">
         <is>
-          <t>07-May-2022</t>
+          <t>12-Aug-2022</t>
         </is>
       </c>
       <c r="DI2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="DK2" t="inlineStr">
@@ -9505,12 +9515,12 @@
       </c>
       <c r="DU2" s="58" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="DV2" s="58" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="DW2" s="53" t="inlineStr">
@@ -9575,7 +9585,7 @@
       </c>
       <c r="EI2" s="58" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="EJ2" s="61" t="n"/>
@@ -9960,12 +9970,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -10690,7 +10700,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="56" t="inlineStr">
@@ -11018,7 +11028,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" s="56" t="inlineStr">
@@ -11034,7 +11044,7 @@
       <c r="F2" s="59" t="n"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="H2" s="59" t="inlineStr">
@@ -11044,12 +11054,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="K2" s="59" t="n"/>
@@ -11249,12 +11259,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" s="58" t="inlineStr">
@@ -11304,14 +11314,14 @@
       <c r="O2" s="59" t="n"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>07-May-2021</t>
+          <t>12-Aug-2021</t>
         </is>
       </c>
       <c r="Q2" s="59" t="n"/>
       <c r="R2" s="59" t="n"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>07-May-2022</t>
+          <t>12-Aug-2022</t>
         </is>
       </c>
     </row>
@@ -11338,8 +11348,8 @@
   </sheetPr>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -11536,17 +11546,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BNS5_26102020092357SDC</t>
+          <t>BNS5_29102020093004BXB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>S5TERM26102020100203HRK</t>
+          <t>S5TERM29102020095338CMU</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>60001303</t>
+          <t>60001334</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -11556,7 +11566,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>04-Sep-2020</t>
+          <t>14-Sep-2021</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -11576,7 +11586,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2520.00</t>
+          <t>36553.43</t>
         </is>
       </c>
       <c r="L2" s="112" t="inlineStr">
@@ -11584,10 +11594,8 @@
           <t>-20.00</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2500.00</t>
-        </is>
+      <c r="M2" t="n">
+        <v>36533.43</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -11601,7 +11609,7 @@
       </c>
       <c r="P2" s="91" t="inlineStr">
         <is>
-          <t>1080.00</t>
+          <t>15665.75</t>
         </is>
       </c>
       <c r="Q2" s="112" t="inlineStr">
@@ -11611,7 +11619,7 @@
       </c>
       <c r="R2" s="91" t="inlineStr">
         <is>
-          <t>1100.00</t>
+          <t>15685.75</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -11650,7 +11658,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>CB001 / Hold for Investment - Australia / BG_COL - Corporate Lending</t>
+          <t>CB001 / Hold for Investment - Australia / BP_COL - Corporate Lending</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -11660,7 +11668,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>CB001/Hold for Investment - Australia/BG_COL</t>
+          <t>CB001/Hold for Investment - Australia/BP_COL</t>
         </is>
       </c>
     </row>

</xml_diff>